<commit_message>
add some doc files
</commit_message>
<xml_diff>
--- a/doc/短线手动交易/交易订单表/交易订单表.xlsx
+++ b/doc/短线手动交易/交易订单表/交易订单表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27948" windowHeight="12300"/>
+    <workbookView windowWidth="25068" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,11 +76,103 @@
       </xdr:spPr>
     </xdr:pic>
   </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="ID_B3BFE9F9F57C4BFAAAFBD10912B104AE" descr="2024年12月7日11点59分_APE_2h"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7772400" cy="3741420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="ID_DB359E07B5434E7285C5CC09CE652F89" descr="2024年12月7日11点59分_ape_5m"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7520940" cy="3877945"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="ID_4DB72D1323F54B198E8130976E782152" descr="2024年12月7日13点47分_ena_5m"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7246620" cy="3763645"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="ID_E45D314EFAA94689A83101B26073FFEB" descr="2024年12月7日13点47分_ena_2h"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8877300" cy="3924300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
 </etc:cellImages>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>开单时间</t>
   </si>
@@ -94,10 +186,10 @@
     <t>杠杆</t>
   </si>
   <si>
-    <t>开单形态（2小时）</t>
-  </si>
-  <si>
-    <t>开单形态（5小时）</t>
+    <t>开单形态（2h）</t>
+  </si>
+  <si>
+    <t>开单形态（5m）</t>
   </si>
   <si>
     <t>开单依据</t>
@@ -106,18 +198,41 @@
     <t>收益(u)</t>
   </si>
   <si>
+    <t>账户余额（u）</t>
+  </si>
+  <si>
     <t>2024年12月6日21点25分</t>
   </si>
   <si>
     <t>NEIROUSDT</t>
-  </si>
-  <si>
-    <t>100u</t>
   </si>
   <si>
     <t>2小时有比较大幅度下跌，有吞没形态
 1小时，2小时macd均出现减弱的迹象，
 处在支撑位，密集成交区</t>
+  </si>
+  <si>
+    <t>2024年12月7日11点59分</t>
+  </si>
+  <si>
+    <t>APEUSDT</t>
+  </si>
+  <si>
+    <t>2小时下方出现支撑位，且有两次测试，且位置处于之前震荡区域的低点
+5分钟前低被抬高，且突破了前低，有回踩迹象，下方出现纺锤形态</t>
+  </si>
+  <si>
+    <t>2024年12月7日13点47分</t>
+  </si>
+  <si>
+    <t>ENAUSDT</t>
+  </si>
+  <si>
+    <t>2小时成很完美的上涨趋势
+5分钟有回踩前低的密集成交区，认为后续也会接着涨，防守前低</t>
+  </si>
+  <si>
+    <t>续前</t>
   </si>
 </sst>
 </file>
@@ -140,13 +255,13 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
       <charset val="134"/>
@@ -305,6 +420,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -419,12 +546,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -462,12 +583,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,7 +737,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -646,16 +761,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -664,78 +779,78 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,7 +861,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,10 +872,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="31" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1073,24 +1209,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="29.4166666666667" customWidth="1"/>
-    <col min="2" max="2" width="18.4907407407407" customWidth="1"/>
-    <col min="3" max="3" width="11.6388888888889" customWidth="1"/>
-    <col min="4" max="4" width="11.4537037037037" customWidth="1"/>
-    <col min="5" max="6" width="25.7777777777778" customWidth="1"/>
-    <col min="7" max="7" width="50.7777777777778" customWidth="1"/>
-    <col min="8" max="8" width="11.4537037037037" customWidth="1"/>
+    <col min="1" max="1" width="23.4907407407407" customWidth="1"/>
+    <col min="2" max="2" width="13.9351851851852" customWidth="1"/>
+    <col min="3" max="3" width="9.86111111111111" customWidth="1"/>
+    <col min="4" max="4" width="7.08333333333333" customWidth="1"/>
+    <col min="5" max="5" width="18.6388888888889" customWidth="1"/>
+    <col min="6" max="6" width="19.1944444444444" customWidth="1"/>
+    <col min="7" max="7" width="40.7777777777778" customWidth="1"/>
+    <col min="8" max="8" width="9.86111111111111" customWidth="1"/>
+    <col min="9" max="9" width="16.5277777777778" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="48.5" customHeight="1" spans="1:8">
+    <row r="1" ht="18.5" customHeight="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,18 +1253,21 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" ht="150" customHeight="1" spans="1:8">
+    <row r="2" ht="110" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
+      <c r="C2" s="2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
         <v>20</v>
       </c>
       <c r="E2" s="2" t="str">
@@ -1137,11 +1278,107 @@
         <f>_xlfn.DISPIMG("ID_E6BD1537F7CC47BE80E3C5C29E1DC25C",1)</f>
         <v>=DISPIMG("ID_E6BD1537F7CC47BE80E3C5C29E1DC25C",1)</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>60</v>
+      </c>
+      <c r="I2" s="6">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" ht="110" customHeight="1" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6">
+        <v>102</v>
+      </c>
+      <c r="D3" s="6">
+        <v>20</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <f>_xlfn.DISPIMG("ID_B3BFE9F9F57C4BFAAAFBD10912B104AE",1)</f>
+        <v>=DISPIMG("ID_B3BFE9F9F57C4BFAAAFBD10912B104AE",1)</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <f>_xlfn.DISPIMG("ID_DB359E07B5434E7285C5CC09CE652F89",1)</f>
+        <v>=DISPIMG("ID_DB359E07B5434E7285C5CC09CE652F89",1)</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="8">
+        <v>-25.23</v>
+      </c>
+      <c r="I3" s="6">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="4" ht="110" customHeight="1" spans="1:9">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6">
+        <v>56</v>
+      </c>
+      <c r="D4" s="6">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="str">
+        <f>_xlfn.DISPIMG("ID_E45D314EFAA94689A83101B26073FFEB",1)</f>
+        <v>=DISPIMG("ID_E45D314EFAA94689A83101B26073FFEB",1)</v>
+      </c>
+      <c r="F4" s="5" t="str">
+        <f>_xlfn.DISPIMG("ID_4DB72D1323F54B198E8130976E782152",1)</f>
+        <v>=DISPIMG("ID_4DB72D1323F54B198E8130976E782152",1)</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="9">
+        <v>11.94</v>
+      </c>
+      <c r="I4" s="6">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="5" ht="110" customHeight="1" spans="1:9">
+      <c r="A5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6">
+        <v>50</v>
+      </c>
+      <c r="D5" s="6">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_98E02948B4094928A9AAF8AC4F23D32E",1)</f>
+        <v>=DISPIMG("ID_98E02948B4094928A9AAF8AC4F23D32E",1)</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_E6BD1537F7CC47BE80E3C5C29E1DC25C",1)</f>
+        <v>=DISPIMG("ID_E6BD1537F7CC47BE80E3C5C29E1DC25C",1)</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="9">
+        <v>74</v>
+      </c>
+      <c r="I5" s="6">
+        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>